<commit_message>
Define flexibility parameter functions
</commit_message>
<xml_diff>
--- a/exports/PackSize-Flexibility/0-RandomVariable.xlsx
+++ b/exports/PackSize-Flexibility/0-RandomVariable.xlsx
@@ -412,10 +412,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.9898477157360406</v>
+        <v>0.9974619289340102</v>
       </c>
       <c r="C2">
-        <v>0.01015228426395939</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1503,10 +1503,10 @@
         <v>0.04568527918781726</v>
       </c>
       <c r="D33">
-        <v>0.04822335025380711</v>
+        <v>0.05076142131979695</v>
       </c>
       <c r="E33">
-        <v>0.01015228426395939</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="F33">
         <v>0.01015228426395939</v>
@@ -1611,10 +1611,10 @@
         <v>0.03045685279187817</v>
       </c>
       <c r="E36">
-        <v>0.01269035532994924</v>
+        <v>0.01522842639593909</v>
       </c>
       <c r="F36">
-        <v>0.002538071065989848</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -2235,10 +2235,10 @@
         <v>0.9390862944162437</v>
       </c>
       <c r="C54">
-        <v>0.03807106598984772</v>
+        <v>0.04060913705583756</v>
       </c>
       <c r="D54">
-        <v>0.01776649746192894</v>
+        <v>0.01522842639593909</v>
       </c>
       <c r="E54">
         <v>0.005076142131979695</v>
@@ -3844,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3967,7 +3967,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -4007,7 +4007,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -4027,7 +4027,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -4039,7 +4039,7 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -4074,7 +4074,7 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -4115,7 +4115,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -4132,31 +4132,31 @@
         <v>27</v>
       </c>
       <c r="B29">
+        <v>0.125</v>
+      </c>
+      <c r="C29">
+        <v>0.125</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0.375</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0.125</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
         <v>0.25</v>
-      </c>
-      <c r="C29">
-        <v>0.25</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0.75</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0.25</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0.5</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -4167,34 +4167,34 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.2857142857142857</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C30">
-        <v>0.2857142857142857</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="D30">
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="E30">
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
         <v>0.1428571428571428</v>
       </c>
-      <c r="E30">
+      <c r="H30">
+        <v>0.2142857142857143</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
         <v>0.1428571428571428</v>
       </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H30">
-        <v>0.4285714285714285</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="J30">
-        <v>0.2857142857142857</v>
-      </c>
       <c r="K30">
-        <v>0.1428571428571428</v>
+        <v>0.07142857142857142</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -4211,25 +4211,25 @@
         <v>0</v>
       </c>
       <c r="E31">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="F31">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <v>0.1333333333333333</v>
       </c>
-      <c r="F31">
-        <v>0.1333333333333333</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0.2666666666666667</v>
-      </c>
       <c r="J31">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="K31">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -4240,31 +4240,31 @@
         <v>0</v>
       </c>
       <c r="C32">
+        <v>0.04761904761904762</v>
+      </c>
+      <c r="D32">
         <v>0.09523809523809523</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>0.1904761904761905</v>
       </c>
-      <c r="E32">
-        <v>0.3809523809523809</v>
-      </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="G32">
-        <v>0.1904761904761905</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32">
-        <v>0.09523809523809523</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="J32">
-        <v>0.4761904761904762</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="K32">
-        <v>0.5714285714285714</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -4278,28 +4278,28 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>0.1818181818181818</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="E33">
-        <v>0.1818181818181818</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="F33">
-        <v>0.09090909090909091</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="G33">
-        <v>0.2727272727272727</v>
+        <v>0.1363636363636364</v>
       </c>
       <c r="H33">
-        <v>0.09090909090909091</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="J33">
-        <v>0.4545454545454545</v>
+        <v>0.2272727272727273</v>
       </c>
       <c r="K33">
-        <v>0.7272727272727273</v>
+        <v>0.3181818181818182</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -4313,28 +4313,28 @@
         <v>0</v>
       </c>
       <c r="D34">
+        <v>0.05</v>
+      </c>
+      <c r="E34">
         <v>0.1</v>
       </c>
-      <c r="E34">
-        <v>0.2</v>
-      </c>
       <c r="F34">
+        <v>0.05</v>
+      </c>
+      <c r="G34">
+        <v>0.05</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
         <v>0.1</v>
       </c>
-      <c r="G34">
-        <v>0.1</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0.2</v>
-      </c>
       <c r="J34">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K34">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -4348,28 +4348,28 @@
         <v>0</v>
       </c>
       <c r="D35">
+        <v>0.05882352941176471</v>
+      </c>
+      <c r="E35">
+        <v>0.05882352941176471</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
         <v>0.1176470588235294</v>
       </c>
-      <c r="E35">
-        <v>0.1176470588235294</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0.2352941176470588</v>
-      </c>
       <c r="J35">
-        <v>1.176470588235294</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="K35">
-        <v>0.3529411764705883</v>
+        <v>0.1764705882352941</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -4377,34 +4377,34 @@
         <v>34</v>
       </c>
       <c r="B36">
+        <v>0.05</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
         <v>0.1</v>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
+      <c r="E36">
+        <v>0.05</v>
+      </c>
+      <c r="F36">
+        <v>0.1</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0.15</v>
+      </c>
+      <c r="I36">
         <v>0.2</v>
       </c>
-      <c r="E36">
-        <v>0.1</v>
-      </c>
-      <c r="F36">
+      <c r="J36">
         <v>0.2</v>
       </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0.3</v>
-      </c>
-      <c r="I36">
-        <v>0.4</v>
-      </c>
-      <c r="J36">
-        <v>0.4</v>
-      </c>
       <c r="K36">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -4415,31 +4415,31 @@
         <v>0</v>
       </c>
       <c r="C37">
+        <v>0.09523809523809523</v>
+      </c>
+      <c r="D37">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="E37">
+        <v>0.09523809523809523</v>
+      </c>
+      <c r="F37">
+        <v>0.04761904761904762</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="J37">
         <v>0.1904761904761905</v>
       </c>
-      <c r="D37">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="E37">
-        <v>0.1904761904761905</v>
-      </c>
-      <c r="F37">
+      <c r="K37">
         <v>0.09523809523809523</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="J37">
-        <v>0.3809523809523809</v>
-      </c>
-      <c r="K37">
-        <v>0.1904761904761905</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -4450,31 +4450,31 @@
         <v>0</v>
       </c>
       <c r="C38">
+        <v>0.08</v>
+      </c>
+      <c r="D38">
+        <v>0.2</v>
+      </c>
+      <c r="E38">
+        <v>0.2</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0.04</v>
+      </c>
+      <c r="H38">
+        <v>0.12</v>
+      </c>
+      <c r="I38">
         <v>0.16</v>
       </c>
-      <c r="D38">
-        <v>0.4</v>
-      </c>
-      <c r="E38">
-        <v>0.4</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
+      <c r="J38">
+        <v>0.12</v>
+      </c>
+      <c r="K38">
         <v>0.08</v>
-      </c>
-      <c r="H38">
-        <v>0.24</v>
-      </c>
-      <c r="I38">
-        <v>0.32</v>
-      </c>
-      <c r="J38">
-        <v>0.24</v>
-      </c>
-      <c r="K38">
-        <v>0.16</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -4482,28 +4482,28 @@
         <v>37</v>
       </c>
       <c r="B39">
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="C39">
+        <v>0.2142857142857143</v>
+      </c>
+      <c r="D39">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="I39">
         <v>0.1428571428571428</v>
-      </c>
-      <c r="C39">
-        <v>0.4285714285714285</v>
-      </c>
-      <c r="D39">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="I39">
-        <v>0.2857142857142857</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -4517,13 +4517,13 @@
         <v>38</v>
       </c>
       <c r="B40">
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="C40">
         <v>0.1428571428571428</v>
       </c>
-      <c r="C40">
-        <v>0.2857142857142857</v>
-      </c>
       <c r="D40">
-        <v>0.4285714285714285</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -4532,16 +4532,16 @@
         <v>0</v>
       </c>
       <c r="G40">
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="H40">
         <v>0.1428571428571428</v>
       </c>
-      <c r="H40">
-        <v>0.2857142857142857</v>
-      </c>
       <c r="I40">
-        <v>0.2857142857142857</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="J40">
-        <v>0.4285714285714285</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -4555,22 +4555,22 @@
         <v>0</v>
       </c>
       <c r="C41">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
         <v>0.6666666666666666</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>1.333333333333333</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -4587,13 +4587,13 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.6153846153846154</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="C42">
-        <v>0.4615384615384616</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="D42">
-        <v>0.3076923076923077</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -4605,10 +4605,10 @@
         <v>0</v>
       </c>
       <c r="H42">
-        <v>0.1538461538461539</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="I42">
-        <v>0.4615384615384616</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -4622,22 +4622,22 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C43">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -4657,25 +4657,25 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C44">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
         <v>0.3333333333333333</v>
       </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0.6666666666666666</v>
-      </c>
       <c r="G44">
         <v>0</v>
       </c>
       <c r="H44">
-        <v>0.3333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -4695,22 +4695,22 @@
         <v>0</v>
       </c>
       <c r="C45">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="F45">
         <v>0.2857142857142857</v>
       </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
+      <c r="G45">
         <v>0.2857142857142857</v>
       </c>
-      <c r="F45">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="G45">
-        <v>0.5714285714285714</v>
-      </c>
       <c r="H45">
-        <v>0.2857142857142857</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -4727,25 +4727,25 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="C46">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H46">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -4771,7 +4771,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -4800,16 +4800,16 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D48">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -4847,7 +4847,7 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -4870,16 +4870,16 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F50">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -4902,7 +4902,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.2857142857142857</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -4911,10 +4911,10 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>0.8571428571428571</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="F51">
-        <v>0.8571428571428571</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -4943,25 +4943,25 @@
         <v>0</v>
       </c>
       <c r="D52">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="E52">
         <v>0.3333333333333333</v>
       </c>
-      <c r="E52">
-        <v>0.6666666666666666</v>
-      </c>
       <c r="F52">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G52">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="H52">
         <v>0</v>
       </c>
       <c r="I52">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="J52">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -4975,16 +4975,16 @@
         <v>0</v>
       </c>
       <c r="C53">
-        <v>0.2222222222222222</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D53">
-        <v>0.1111111111111111</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="E53">
-        <v>0.7777777777777778</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="F53">
-        <v>0.7777777777777778</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -4993,7 +4993,7 @@
         <v>0</v>
       </c>
       <c r="I53">
-        <v>0.1111111111111111</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -5007,19 +5007,19 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.09523809523809523</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>0.1904761904761905</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="E54">
-        <v>0.9523809523809523</v>
+        <v>0.4761904761904762</v>
       </c>
       <c r="F54">
-        <v>0.09523809523809523</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -5028,13 +5028,13 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>0.3809523809523809</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="J54">
         <v>0</v>
       </c>
       <c r="K54">
-        <v>0.2857142857142857</v>
+        <v>0.1428571428571428</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -5045,13 +5045,13 @@
         <v>0</v>
       </c>
       <c r="C55">
+        <v>0.1176470588235294</v>
+      </c>
+      <c r="D55">
         <v>0.2352941176470588</v>
       </c>
-      <c r="D55">
-        <v>0.4705882352941176</v>
-      </c>
       <c r="E55">
-        <v>0.8235294117647058</v>
+        <v>0.4117647058823529</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -5060,13 +5060,13 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <v>0.2352941176470588</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="I55">
-        <v>0.1176470588235294</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="J55">
-        <v>0.1176470588235294</v>
+        <v>0.05882352941176471</v>
       </c>
       <c r="K55">
         <v>0</v>
@@ -5077,31 +5077,31 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E56">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F56">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="G56">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="H56">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="I56">
         <v>0</v>
       </c>
       <c r="J56">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -5115,16 +5115,16 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <v>0.3636363636363636</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="D57">
-        <v>0.5454545454545454</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="E57">
-        <v>0.5454545454545454</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="F57">
-        <v>0.3636363636363636</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -5133,7 +5133,7 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <v>0.1818181818181818</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="J57">
         <v>0</v>
@@ -5150,13 +5150,13 @@
         <v>0</v>
       </c>
       <c r="C58">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D58">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E58">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -5182,13 +5182,13 @@
         <v>57</v>
       </c>
       <c r="B59">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="C59">
+        <v>0.5</v>
+      </c>
+      <c r="D59">
         <v>0.3333333333333333</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>0.6666666666666666</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -5223,13 +5223,13 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E60">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F60">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -5252,16 +5252,16 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="C61">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="E61">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -5292,10 +5292,10 @@
         <v>61</v>
       </c>
       <c r="B63">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="C63">
         <v>0.6666666666666666</v>
-      </c>
-      <c r="C63">
-        <v>1.333333333333333</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -5330,7 +5330,7 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -5367,7 +5367,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -5407,13 +5407,13 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -5462,7 +5462,7 @@
         <v>0</v>
       </c>
       <c r="G70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -5512,7 +5512,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -5552,7 +5552,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -5595,7 +5595,7 @@
         <v>0</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -5630,7 +5630,7 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -5694,7 +5694,7 @@
         <v>0</v>
       </c>
       <c r="K84">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -5722,7 +5722,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -5775,7 +5775,7 @@
         <v>0</v>
       </c>
       <c r="H90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I90">
         <v>0</v>
@@ -5872,13 +5872,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -5907,7 +5907,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -5942,7 +5942,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5977,7 +5977,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5986,7 +5986,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -6012,7 +6012,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -6047,7 +6047,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -6082,7 +6082,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -6117,7 +6117,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -6152,7 +6152,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -6187,7 +6187,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -6222,7 +6222,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -6257,7 +6257,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -6292,7 +6292,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -6327,7 +6327,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -6362,7 +6362,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -6397,7 +6397,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -6432,7 +6432,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -6467,13 +6467,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -6502,7 +6502,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -6537,7 +6537,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -6572,7 +6572,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -6607,10 +6607,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C23">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -6642,7 +6642,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -6677,10 +6677,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C25">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -6712,10 +6712,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C26">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -6747,10 +6747,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0.1658206429780034</v>
+        <v>0.9949238578680202</v>
       </c>
       <c r="C27">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -6782,7 +6782,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -6817,13 +6817,13 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0.1641285956006768</v>
+        <v>0.984771573604061</v>
       </c>
       <c r="C29">
-        <v>0.001692047377326565</v>
+        <v>0.01015228426395939</v>
       </c>
       <c r="D29">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -6852,13 +6852,13 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.1611675126903553</v>
+        <v>0.967005076142132</v>
       </c>
       <c r="C30">
-        <v>0.004230118443316413</v>
+        <v>0.02538071065989848</v>
       </c>
       <c r="D30">
-        <v>0.001269035532994924</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -6887,19 +6887,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0.1594754653130288</v>
+        <v>0.9568527918781726</v>
       </c>
       <c r="C31">
-        <v>0.005499153976311336</v>
+        <v>0.03299492385786802</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="F31">
-        <v>0.001269035532994924</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -6922,19 +6922,19 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.1552453468697123</v>
+        <v>0.931472081218274</v>
       </c>
       <c r="C32">
-        <v>0.007614213197969543</v>
+        <v>0.04568527918781726</v>
       </c>
       <c r="D32">
+        <v>0.01522842639593909</v>
+      </c>
+      <c r="E32">
+        <v>0.005076142131979695</v>
+      </c>
+      <c r="F32">
         <v>0.002538071065989848</v>
-      </c>
-      <c r="E32">
-        <v>0.0008460236886632825</v>
-      </c>
-      <c r="F32">
-        <v>0.0004230118443316413</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -6957,25 +6957,25 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.1489001692047377</v>
+        <v>0.8934010152284264</v>
       </c>
       <c r="C33">
-        <v>0.00676818950930626</v>
+        <v>0.04060913705583756</v>
       </c>
       <c r="D33">
-        <v>0.00338409475465313</v>
+        <v>0.02030456852791878</v>
       </c>
       <c r="E33">
-        <v>0.003807106598984772</v>
+        <v>0.02284263959390863</v>
       </c>
       <c r="F33">
-        <v>0.002115059221658206</v>
+        <v>0.01269035532994924</v>
       </c>
       <c r="G33">
-        <v>0.001269035532994924</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="H33">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -6992,25 +6992,25 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.149746192893401</v>
+        <v>0.8984771573604061</v>
       </c>
       <c r="C34">
-        <v>0.005922165820642978</v>
+        <v>0.03553299492385787</v>
       </c>
       <c r="D34">
-        <v>0.004230118443316413</v>
+        <v>0.02538071065989848</v>
       </c>
       <c r="E34">
-        <v>0.002961082910321489</v>
+        <v>0.01776649746192894</v>
       </c>
       <c r="F34">
-        <v>0.001269035532994924</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="G34">
-        <v>0.002115059221658206</v>
+        <v>0.01269035532994924</v>
       </c>
       <c r="H34">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -7027,22 +7027,22 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0.1539763113367174</v>
+        <v>0.9238578680203045</v>
       </c>
       <c r="C35">
+        <v>0.03045685279187817</v>
+      </c>
+      <c r="D35">
+        <v>0.02284263959390863</v>
+      </c>
+      <c r="E35">
+        <v>0.01269035532994924</v>
+      </c>
+      <c r="F35">
         <v>0.005076142131979695</v>
       </c>
-      <c r="D35">
-        <v>0.003807106598984772</v>
-      </c>
-      <c r="E35">
-        <v>0.002115059221658206</v>
-      </c>
-      <c r="F35">
-        <v>0.0008460236886632825</v>
-      </c>
       <c r="G35">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -7062,28 +7062,28 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0.1543993231810491</v>
+        <v>0.9263959390862944</v>
       </c>
       <c r="C36">
+        <v>0.01522842639593909</v>
+      </c>
+      <c r="D36">
+        <v>0.02791878172588833</v>
+      </c>
+      <c r="E36">
+        <v>0.01522842639593909</v>
+      </c>
+      <c r="F36">
+        <v>0.01015228426395939</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
         <v>0.002538071065989848</v>
       </c>
-      <c r="D36">
-        <v>0.004653130287648054</v>
-      </c>
-      <c r="E36">
+      <c r="I36">
         <v>0.002538071065989848</v>
-      </c>
-      <c r="F36">
-        <v>0.001692047377326565</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0.0004230118443316413</v>
-      </c>
-      <c r="I36">
-        <v>0.0004230118443316413</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -7097,22 +7097,22 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0.1577834179357022</v>
+        <v>0.9467005076142132</v>
       </c>
       <c r="C37">
-        <v>0.004230118443316413</v>
+        <v>0.02538071065989848</v>
       </c>
       <c r="D37">
-        <v>0.002961082910321489</v>
+        <v>0.01776649746192894</v>
       </c>
       <c r="E37">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="F37">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="G37">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -7132,25 +7132,25 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0.1577834179357022</v>
+        <v>0.9467005076142132</v>
       </c>
       <c r="C38">
-        <v>0.004653130287648054</v>
+        <v>0.02791878172588833</v>
       </c>
       <c r="D38">
+        <v>0.01522842639593909</v>
+      </c>
+      <c r="E38">
+        <v>0.007614213197969543</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
         <v>0.002538071065989848</v>
-      </c>
-      <c r="E38">
-        <v>0.001269035532994924</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0.0004230118443316413</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -7167,16 +7167,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.1624365482233502</v>
+        <v>0.9746192893401014</v>
       </c>
       <c r="C39">
-        <v>0.002961082910321489</v>
+        <v>0.01776649746192894</v>
       </c>
       <c r="D39">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E39">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -7202,16 +7202,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.1611675126903553</v>
+        <v>0.967005076142132</v>
       </c>
       <c r="C40">
-        <v>0.002538071065989848</v>
+        <v>0.01522842639593909</v>
       </c>
       <c r="D40">
-        <v>0.002115059221658206</v>
+        <v>0.01269035532994924</v>
       </c>
       <c r="E40">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -7237,13 +7237,13 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0.1653976311336718</v>
+        <v>0.9923857868020305</v>
       </c>
       <c r="C41">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D41">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -7252,7 +7252,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -7272,10 +7272,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.1632825719120135</v>
+        <v>0.9796954314720812</v>
       </c>
       <c r="C42">
-        <v>0.00338409475465313</v>
+        <v>0.02030456852791878</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -7307,13 +7307,13 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.1653976311336718</v>
+        <v>0.9923857868020305</v>
       </c>
       <c r="C43">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D43">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -7342,13 +7342,13 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0.1653976311336718</v>
+        <v>0.9923857868020305</v>
       </c>
       <c r="C44">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="D44">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -7377,13 +7377,13 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0.1649746192893401</v>
+        <v>0.9898477157360406</v>
       </c>
       <c r="C45">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="D45">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -7412,13 +7412,13 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.1649746192893401</v>
+        <v>0.9898477157360406</v>
       </c>
       <c r="C46">
-        <v>0.001269035532994924</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="D46">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -7447,10 +7447,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C47">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -7482,13 +7482,13 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0.1649746192893401</v>
+        <v>0.9898477157360406</v>
       </c>
       <c r="C48">
-        <v>0.001269035532994924</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="D48">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -7517,10 +7517,10 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C49">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -7552,10 +7552,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0.1658206429780034</v>
+        <v>0.9949238578680202</v>
       </c>
       <c r="C50">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -7587,10 +7587,10 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C51">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -7622,10 +7622,10 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0.1653976311336718</v>
+        <v>0.9923857868020305</v>
       </c>
       <c r="C52">
-        <v>0.001269035532994924</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -7657,13 +7657,13 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.1649746192893401</v>
+        <v>0.9898477157360406</v>
       </c>
       <c r="C53">
-        <v>0.001269035532994924</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="D53">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -7692,16 +7692,16 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.1607445008460237</v>
+        <v>0.9644670050761422</v>
       </c>
       <c r="C54">
-        <v>0.003807106598984772</v>
+        <v>0.02284263959390863</v>
       </c>
       <c r="D54">
-        <v>0.001692047377326565</v>
+        <v>0.01015228426395939</v>
       </c>
       <c r="E54">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -7727,13 +7727,13 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.1628595600676819</v>
+        <v>0.9771573604060915</v>
       </c>
       <c r="C55">
-        <v>0.002115059221658206</v>
+        <v>0.01269035532994924</v>
       </c>
       <c r="D55">
-        <v>0.001692047377326565</v>
+        <v>0.01015228426395939</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -7762,13 +7762,13 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0.1637055837563452</v>
+        <v>0.9822335025380711</v>
       </c>
       <c r="C56">
+        <v>0.01522842639593909</v>
+      </c>
+      <c r="D56">
         <v>0.002538071065989848</v>
-      </c>
-      <c r="D56">
-        <v>0.0004230118443316413</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -7797,16 +7797,16 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.1653976311336718</v>
+        <v>0.9923857868020305</v>
       </c>
       <c r="C57">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D57">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E57">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -7832,10 +7832,10 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.1658206429780034</v>
+        <v>0.9949238578680202</v>
       </c>
       <c r="C58">
-        <v>0.0008460236886632825</v>
+        <v>0.005076142131979695</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -7867,13 +7867,13 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.1649746192893401</v>
+        <v>0.9898477157360406</v>
       </c>
       <c r="C59">
-        <v>0.001269035532994924</v>
+        <v>0.007614213197969543</v>
       </c>
       <c r="D59">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -7902,13 +7902,13 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0.1658206429780034</v>
+        <v>0.9949238578680202</v>
       </c>
       <c r="C60">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D60">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -7937,13 +7937,13 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.1658206429780034</v>
+        <v>0.9949238578680202</v>
       </c>
       <c r="C61">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D61">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -7972,7 +7972,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -8007,13 +8007,13 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.1658206429780034</v>
+        <v>0.9949238578680202</v>
       </c>
       <c r="C63">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D63">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -8042,10 +8042,10 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C64">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -8077,7 +8077,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -8112,10 +8112,10 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C66">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -8147,7 +8147,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -8182,10 +8182,10 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C68">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -8217,7 +8217,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -8252,7 +8252,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -8287,7 +8287,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -8322,7 +8322,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -8357,7 +8357,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -8392,7 +8392,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -8427,7 +8427,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -8462,7 +8462,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -8497,7 +8497,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -8532,7 +8532,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -8567,7 +8567,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -8602,7 +8602,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -8637,13 +8637,13 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -8672,10 +8672,10 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C82">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -8707,7 +8707,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -8742,7 +8742,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -8751,7 +8751,7 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -8777,7 +8777,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -8812,7 +8812,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -8847,7 +8847,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -8882,7 +8882,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -8917,7 +8917,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -8952,13 +8952,13 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0.166243654822335</v>
+        <v>0.9974619289340101</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>0.0004230118443316413</v>
+        <v>0.002538071065989848</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -8987,7 +8987,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -9022,7 +9022,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -9057,7 +9057,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -9092,7 +9092,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -9127,7 +9127,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -9162,7 +9162,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -9197,7 +9197,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -9280,7 +9280,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>9.999999999999996</v>
+        <v>0.9999999999999997</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -9349,7 +9349,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -9425,7 +9425,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>9.999999999999996</v>
+        <v>0.9999999999999997</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -9478,7 +9478,7 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>5.000000000000001</v>
+        <v>0.5000000000000001</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -9499,7 +9499,7 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>4.999999999999996</v>
+        <v>0.4999999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -9515,7 +9515,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>4.999999999999998</v>
+        <v>0.4999999999999998</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -9524,7 +9524,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>5.000000000000001</v>
+        <v>0.5000000000000001</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -9553,7 +9553,7 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>5.000000000000001</v>
+        <v>0.5000000000000001</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -9574,7 +9574,7 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>4.999999999999996</v>
+        <v>0.4999999999999996</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -9582,13 +9582,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.333333333333333</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="C27">
-        <v>3.333333333333332</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D27">
-        <v>3.333333333333334</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -9617,13 +9617,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>5.000000000000001</v>
+        <v>0.5000000000000001</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -9655,16 +9655,16 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>4.999999999999998</v>
+        <v>0.4999999999999998</v>
       </c>
       <c r="D29">
-        <v>1.25</v>
+        <v>0.125</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>1.25</v>
+        <v>0.125</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -9679,7 +9679,7 @@
         <v>0</v>
       </c>
       <c r="K29">
-        <v>2.499999999999998</v>
+        <v>0.2499999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -9687,13 +9687,13 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.6666666666666666</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C30">
-        <v>2.666666666666666</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="D30">
-        <v>1.333333333333333</v>
+        <v>0.1333333333333334</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -9702,19 +9702,19 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <v>0.6666666666666661</v>
+        <v>0.06666666666666661</v>
       </c>
       <c r="H30">
-        <v>1.333333333333333</v>
+        <v>0.1333333333333334</v>
       </c>
       <c r="I30">
-        <v>0.6666666666666667</v>
+        <v>0.06666666666666668</v>
       </c>
       <c r="J30">
         <v>0</v>
       </c>
       <c r="K30">
-        <v>2.666666666666664</v>
+        <v>0.2666666666666664</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -9722,19 +9722,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>1.5</v>
+        <v>0.15</v>
       </c>
       <c r="C31">
-        <v>4.499999999999998</v>
+        <v>0.4499999999999998</v>
       </c>
       <c r="D31">
-        <v>2.500000000000001</v>
+        <v>0.2500000000000001</v>
       </c>
       <c r="E31">
-        <v>0.5000000000000001</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="F31">
-        <v>0.5000000000000001</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -9746,7 +9746,7 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0.5000000000000001</v>
+        <v>0.05000000000000002</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -9757,34 +9757,34 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.6896551724137931</v>
+        <v>0.06896551724137932</v>
       </c>
       <c r="C32">
-        <v>3.448275862068964</v>
+        <v>0.3448275862068965</v>
       </c>
       <c r="D32">
-        <v>1.724137931034483</v>
+        <v>0.1724137931034483</v>
       </c>
       <c r="E32">
-        <v>0.6896551724137933</v>
+        <v>0.06896551724137932</v>
       </c>
       <c r="F32">
-        <v>1.379310344827587</v>
+        <v>0.1379310344827586</v>
       </c>
       <c r="G32">
-        <v>0.3448275862068962</v>
+        <v>0.03448275862068963</v>
       </c>
       <c r="H32">
-        <v>0.6896551724137933</v>
+        <v>0.06896551724137932</v>
       </c>
       <c r="I32">
-        <v>0.3448275862068966</v>
+        <v>0.03448275862068966</v>
       </c>
       <c r="J32">
         <v>0</v>
       </c>
       <c r="K32">
-        <v>0.6896551724137925</v>
+        <v>0.06896551724137925</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -9792,22 +9792,22 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0.6818181818181818</v>
+        <v>0.06818181818181818</v>
       </c>
       <c r="C33">
-        <v>2.954545454545453</v>
+        <v>0.2954545454545454</v>
       </c>
       <c r="D33">
-        <v>2.5</v>
+        <v>0.2500000000000001</v>
       </c>
       <c r="E33">
-        <v>2.045454545454546</v>
+        <v>0.2045454545454546</v>
       </c>
       <c r="F33">
-        <v>0.9090909090909093</v>
+        <v>0.09090909090909094</v>
       </c>
       <c r="G33">
-        <v>0.6818181818181812</v>
+        <v>0.06818181818181812</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -9816,7 +9816,7 @@
         <v>0</v>
       </c>
       <c r="J33">
-        <v>0.2272727272727273</v>
+        <v>0.02272727272727273</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -9827,22 +9827,22 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0.4545454545454545</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="C34">
-        <v>2.954545454545453</v>
+        <v>0.2954545454545454</v>
       </c>
       <c r="D34">
-        <v>4.090909090909092</v>
+        <v>0.4090909090909092</v>
       </c>
       <c r="E34">
-        <v>1.590909090909091</v>
+        <v>0.1590909090909091</v>
       </c>
       <c r="F34">
-        <v>0.4545454545454546</v>
+        <v>0.04545454545454547</v>
       </c>
       <c r="G34">
-        <v>0.2272727272727271</v>
+        <v>0.02272727272727271</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -9854,7 +9854,7 @@
         <v>0</v>
       </c>
       <c r="K34">
-        <v>0.2272727272727271</v>
+        <v>0.02272727272727271</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -9865,19 +9865,19 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>2.258064516129031</v>
+        <v>0.2258064516129031</v>
       </c>
       <c r="D35">
-        <v>2.903225806451613</v>
+        <v>0.2903225806451614</v>
       </c>
       <c r="E35">
-        <v>2.903225806451613</v>
+        <v>0.2903225806451614</v>
       </c>
       <c r="F35">
-        <v>0.9677419354838712</v>
+        <v>0.09677419354838712</v>
       </c>
       <c r="G35">
-        <v>0.9677419354838702</v>
+        <v>0.09677419354838702</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -9897,25 +9897,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>1.142857142857143</v>
+        <v>0.1142857142857143</v>
       </c>
       <c r="C36">
-        <v>0.8571428571428569</v>
+        <v>0.08571428571428569</v>
       </c>
       <c r="D36">
-        <v>1.428571428571429</v>
+        <v>0.1428571428571429</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="F36">
-        <v>2.571428571428572</v>
+        <v>0.2571428571428572</v>
       </c>
       <c r="G36">
-        <v>1.428571428571427</v>
+        <v>0.1428571428571427</v>
       </c>
       <c r="H36">
-        <v>0.2857142857142858</v>
+        <v>0.02857142857142858</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -9924,7 +9924,7 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>0.2857142857142855</v>
+        <v>0.02857142857142855</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -9932,34 +9932,34 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1.2</v>
+        <v>0.12</v>
       </c>
       <c r="C37">
-        <v>1.599999999999999</v>
+        <v>0.1599999999999999</v>
       </c>
       <c r="D37">
-        <v>0.8000000000000002</v>
+        <v>0.08000000000000002</v>
       </c>
       <c r="E37">
-        <v>0.8000000000000002</v>
+        <v>0.08000000000000002</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="G37">
-        <v>1.599999999999999</v>
+        <v>0.1599999999999999</v>
       </c>
       <c r="H37">
-        <v>0.4000000000000001</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="I37">
-        <v>0.4000000000000001</v>
+        <v>0.04000000000000001</v>
       </c>
       <c r="J37">
         <v>0</v>
       </c>
       <c r="K37">
-        <v>1.199999999999999</v>
+        <v>0.1199999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -9967,25 +9967,25 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>1.612903225806452</v>
+        <v>0.1612903225806452</v>
       </c>
       <c r="C38">
-        <v>2.258064516129031</v>
+        <v>0.2258064516129031</v>
       </c>
       <c r="D38">
-        <v>1.612903225806452</v>
+        <v>0.1612903225806452</v>
       </c>
       <c r="E38">
-        <v>1.612903225806452</v>
+        <v>0.1612903225806452</v>
       </c>
       <c r="F38">
-        <v>1.935483870967742</v>
+        <v>0.1935483870967742</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>0.6451612903225807</v>
+        <v>0.06451612903225808</v>
       </c>
       <c r="I38">
         <v>0</v>
@@ -9994,7 +9994,7 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <v>0.32258064516129</v>
+        <v>0.032258064516129</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -10002,34 +10002,34 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0.6666666666666666</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C39">
-        <v>0.6666666666666664</v>
+        <v>0.06666666666666664</v>
       </c>
       <c r="D39">
-        <v>1.333333333333333</v>
+        <v>0.1333333333333334</v>
       </c>
       <c r="E39">
-        <v>0.6666666666666667</v>
+        <v>0.06666666666666668</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="G39">
-        <v>0.6666666666666661</v>
+        <v>0.06666666666666661</v>
       </c>
       <c r="H39">
-        <v>1.333333333333333</v>
+        <v>0.1333333333333334</v>
       </c>
       <c r="I39">
-        <v>0.6666666666666667</v>
+        <v>0.06666666666666668</v>
       </c>
       <c r="J39">
         <v>0</v>
       </c>
       <c r="K39">
-        <v>1.999999999999998</v>
+        <v>0.1999999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -10037,22 +10037,22 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.6666666666666666</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="C40">
-        <v>1.333333333333333</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="E40">
-        <v>1.333333333333333</v>
+        <v>0.1333333333333334</v>
       </c>
       <c r="F40">
-        <v>0.6666666666666667</v>
+        <v>0.06666666666666668</v>
       </c>
       <c r="G40">
-        <v>0.6666666666666661</v>
+        <v>0.06666666666666661</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -10064,7 +10064,7 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <v>3.33333333333333</v>
+        <v>0.333333333333333</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -10075,16 +10075,16 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>2.499999999999999</v>
+        <v>0.2499999999999999</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>5.000000000000001</v>
+        <v>0.5000000000000001</v>
       </c>
       <c r="F41">
-        <v>2.5</v>
+        <v>0.2500000000000001</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -10107,22 +10107,22 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0.7692307692307693</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="C42">
-        <v>1.538461538461538</v>
+        <v>0.1538461538461538</v>
       </c>
       <c r="D42">
-        <v>0.7692307692307694</v>
+        <v>0.07692307692307694</v>
       </c>
       <c r="E42">
-        <v>0.7692307692307694</v>
+        <v>0.07692307692307694</v>
       </c>
       <c r="F42">
-        <v>1.538461538461539</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="G42">
-        <v>0.7692307692307685</v>
+        <v>0.07692307692307686</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -10134,7 +10134,7 @@
         <v>0</v>
       </c>
       <c r="K42">
-        <v>3.846153846153843</v>
+        <v>0.3846153846153843</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -10151,13 +10151,13 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>1.999999999999998</v>
+        <v>0.1999999999999998</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -10169,7 +10169,7 @@
         <v>0</v>
       </c>
       <c r="K43">
-        <v>5.999999999999995</v>
+        <v>0.5999999999999995</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -10180,10 +10180,10 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>1.666666666666666</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="D44">
-        <v>1.666666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -10195,7 +10195,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>1.666666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -10204,7 +10204,7 @@
         <v>0</v>
       </c>
       <c r="K44">
-        <v>4.999999999999996</v>
+        <v>0.4999999999999996</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -10215,31 +10215,31 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>2.499999999999999</v>
+        <v>0.2499999999999999</v>
       </c>
       <c r="D45">
-        <v>1.25</v>
+        <v>0.125</v>
       </c>
       <c r="E45">
-        <v>1.25</v>
+        <v>0.125</v>
       </c>
       <c r="F45">
-        <v>1.25</v>
+        <v>0.125</v>
       </c>
       <c r="G45">
-        <v>1.249999999999999</v>
+        <v>0.1249999999999999</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45">
-        <v>1.25</v>
+        <v>0.125</v>
       </c>
       <c r="J45">
         <v>0</v>
       </c>
       <c r="K45">
-        <v>1.249999999999999</v>
+        <v>0.1249999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -10250,19 +10250,19 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>1.999999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
-        <v>1.999999999999998</v>
+        <v>0.1999999999999998</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -10274,7 +10274,7 @@
         <v>0</v>
       </c>
       <c r="K46">
-        <v>3.999999999999996</v>
+        <v>0.3999999999999997</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -10303,7 +10303,7 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -10323,13 +10323,13 @@
         <v>0</v>
       </c>
       <c r="D48">
-        <v>2.5</v>
+        <v>0.2500000000000001</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>2.5</v>
+        <v>0.2500000000000001</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -10344,7 +10344,7 @@
         <v>0</v>
       </c>
       <c r="K48">
-        <v>4.999999999999996</v>
+        <v>0.4999999999999996</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -10361,7 +10361,7 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -10387,10 +10387,10 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="C50">
-        <v>1.999999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -10402,10 +10402,10 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>3.999999999999996</v>
+        <v>0.3999999999999997</v>
       </c>
       <c r="H50">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="I50">
         <v>0</v>
@@ -10422,19 +10422,19 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>3.333333333333333</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
       <c r="D51">
-        <v>3.333333333333334</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="E51">
-        <v>1.666666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F51">
-        <v>1.666666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -10457,25 +10457,25 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="C52">
-        <v>0.7142857142857141</v>
+        <v>0.07142857142857141</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>1.428571428571429</v>
+        <v>0.1428571428571429</v>
       </c>
       <c r="F52">
         <v>0</v>
       </c>
       <c r="G52">
-        <v>0.7142857142857136</v>
+        <v>0.07142857142857137</v>
       </c>
       <c r="H52">
-        <v>0.7142857142857144</v>
+        <v>0.07142857142857144</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -10484,7 +10484,7 @@
         <v>0</v>
       </c>
       <c r="K52">
-        <v>1.428571428571427</v>
+        <v>0.1428571428571427</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -10492,25 +10492,25 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>2.352941176470588</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="C53">
-        <v>1.76470588235294</v>
+        <v>0.176470588235294</v>
       </c>
       <c r="D53">
-        <v>2.352941176470589</v>
+        <v>0.2352941176470589</v>
       </c>
       <c r="E53">
-        <v>1.176470588235294</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F53">
-        <v>1.176470588235294</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
-        <v>0.5882352941176472</v>
+        <v>0.05882352941176472</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -10519,7 +10519,7 @@
         <v>0</v>
       </c>
       <c r="K53">
-        <v>0.5882352941176465</v>
+        <v>0.05882352941176466</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -10527,22 +10527,22 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>1.25</v>
+        <v>0.08333333333333334</v>
       </c>
       <c r="C54">
-        <v>1.25</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="D54">
-        <v>3.75</v>
+        <v>0.3750000000000001</v>
       </c>
       <c r="E54">
-        <v>0.8333333333333335</v>
+        <v>0.08333333333333336</v>
       </c>
       <c r="F54">
-        <v>1.666666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="G54">
-        <v>0.4166666666666663</v>
+        <v>0.04166666666666663</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -10554,7 +10554,7 @@
         <v>0</v>
       </c>
       <c r="K54">
-        <v>0.8333333333333326</v>
+        <v>0.08333333333333326</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -10562,25 +10562,25 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0.7142857142857143</v>
+        <v>0.07142857142857144</v>
       </c>
       <c r="C55">
-        <v>2.142857142857142</v>
+        <v>0.2142857142857142</v>
       </c>
       <c r="D55">
-        <v>0.7142857142857144</v>
+        <v>0.07142857142857144</v>
       </c>
       <c r="E55">
-        <v>1.428571428571429</v>
+        <v>0.1428571428571429</v>
       </c>
       <c r="F55">
-        <v>1.428571428571429</v>
+        <v>0.1428571428571429</v>
       </c>
       <c r="G55">
-        <v>2.142857142857141</v>
+        <v>0.2142857142857141</v>
       </c>
       <c r="H55">
-        <v>0.7142857142857144</v>
+        <v>0.07142857142857144</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -10589,7 +10589,7 @@
         <v>0</v>
       </c>
       <c r="K55">
-        <v>0.7142857142857136</v>
+        <v>0.07142857142857137</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -10600,22 +10600,22 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>1.666666666666666</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="D56">
-        <v>0.8333333333333335</v>
+        <v>0.08333333333333336</v>
       </c>
       <c r="E56">
-        <v>2.5</v>
+        <v>0.2500000000000001</v>
       </c>
       <c r="F56">
-        <v>1.666666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="G56">
         <v>0</v>
       </c>
       <c r="H56">
-        <v>0.8333333333333335</v>
+        <v>0.08333333333333336</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -10624,7 +10624,7 @@
         <v>0</v>
       </c>
       <c r="K56">
-        <v>2.499999999999998</v>
+        <v>0.2499999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -10635,13 +10635,13 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <v>2.499999999999999</v>
+        <v>0.2499999999999999</v>
       </c>
       <c r="D57">
-        <v>4.166666666666668</v>
+        <v>0.4166666666666668</v>
       </c>
       <c r="E57">
-        <v>0.8333333333333335</v>
+        <v>0.08333333333333336</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -10650,7 +10650,7 @@
         <v>0</v>
       </c>
       <c r="H57">
-        <v>0.8333333333333335</v>
+        <v>0.08333333333333336</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -10659,7 +10659,7 @@
         <v>0</v>
       </c>
       <c r="K57">
-        <v>1.666666666666665</v>
+        <v>0.1666666666666665</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -10670,22 +10670,22 @@
         <v>0</v>
       </c>
       <c r="C58">
-        <v>1.999999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -10694,7 +10694,7 @@
         <v>0</v>
       </c>
       <c r="K58">
-        <v>1.999999999999998</v>
+        <v>0.1999999999999998</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -10714,7 +10714,7 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>1.666666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -10723,13 +10723,13 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>1.666666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="J59">
         <v>0</v>
       </c>
       <c r="K59">
-        <v>6.666666666666661</v>
+        <v>0.6666666666666661</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -10740,7 +10740,7 @@
         <v>0</v>
       </c>
       <c r="C60">
-        <v>2.499999999999999</v>
+        <v>0.2499999999999999</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -10752,7 +10752,7 @@
         <v>0</v>
       </c>
       <c r="G60">
-        <v>4.999999999999996</v>
+        <v>0.4999999999999996</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -10764,7 +10764,7 @@
         <v>0</v>
       </c>
       <c r="K60">
-        <v>2.499999999999998</v>
+        <v>0.2499999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -10772,7 +10772,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>2.5</v>
+        <v>0.25</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -10790,7 +10790,7 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>2.5</v>
+        <v>0.2500000000000001</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -10799,7 +10799,7 @@
         <v>0</v>
       </c>
       <c r="K61">
-        <v>4.999999999999996</v>
+        <v>0.4999999999999996</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -10833,13 +10833,13 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <v>2.5</v>
+        <v>0.2500000000000001</v>
       </c>
       <c r="J63">
         <v>0</v>
       </c>
       <c r="K63">
-        <v>7.499999999999994</v>
+        <v>0.7499999999999994</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -10874,7 +10874,7 @@
         <v>0</v>
       </c>
       <c r="K64">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -10914,7 +10914,7 @@
         <v>0</v>
       </c>
       <c r="K66">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -10948,13 +10948,13 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <v>5.000000000000001</v>
+        <v>0.5000000000000001</v>
       </c>
       <c r="J68">
         <v>0</v>
       </c>
       <c r="K68">
-        <v>4.999999999999996</v>
+        <v>0.4999999999999996</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -10989,7 +10989,7 @@
         <v>0</v>
       </c>
       <c r="K69">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -11003,7 +11003,7 @@
         <v>0</v>
       </c>
       <c r="D70">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -11079,7 +11079,7 @@
         <v>0</v>
       </c>
       <c r="K75">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -11119,7 +11119,7 @@
         <v>0</v>
       </c>
       <c r="K77">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -11159,7 +11159,7 @@
         <v>0</v>
       </c>
       <c r="K79">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -11194,7 +11194,7 @@
         <v>0</v>
       </c>
       <c r="K80">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -11229,7 +11229,7 @@
         <v>0</v>
       </c>
       <c r="K81">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -11264,7 +11264,7 @@
         <v>0</v>
       </c>
       <c r="K82">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -11286,7 +11286,7 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -11359,7 +11359,7 @@
         <v>0</v>
       </c>
       <c r="K89">
-        <v>9.999999999999991</v>
+        <v>0.9999999999999991</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -11379,7 +11379,7 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G90">
         <v>0</v>

</xml_diff>